<commit_message>
Updated LZ4, Catch and OpenSSL
</commit_message>
<xml_diff>
--- a/Install/Files/Third Party Licenses.xlsx
+++ b/Install/Files/Third Party Licenses.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Project\Install\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E072151A-3A47-4F52-AD86-7095785AD48E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B552BEDB-E6BB-4A8F-AFAA-A8C726C03D9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="17220" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="630" windowWidth="16920" windowHeight="17370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>License</t>
   </si>
@@ -102,33 +102,15 @@
     <t>Qt</t>
   </si>
   <si>
-    <t>Visual Studio 2017 (15.4.2) Runtimes</t>
-  </si>
-  <si>
-    <t>14.11.25325.0</t>
-  </si>
-  <si>
     <t>https://go.microsoft.com/fwlink/?LinkId=746572</t>
   </si>
   <si>
     <t>Free for any use</t>
   </si>
   <si>
-    <t>stb_image</t>
-  </si>
-  <si>
-    <t>Image loading/decoding/encoding/saving</t>
-  </si>
-  <si>
-    <t>https://github.com/nothings/stb</t>
-  </si>
-  <si>
     <t>https://lz4.github.io/lz4/</t>
   </si>
   <si>
-    <t>1.8.2</t>
-  </si>
-  <si>
     <t>The Qt Company</t>
   </si>
   <si>
@@ -174,9 +156,6 @@
     <t>Cryptography and SSL/TLS Toolkit</t>
   </si>
   <si>
-    <t>1.1.0h</t>
-  </si>
-  <si>
     <t>OpenSSL Software Foundation</t>
   </si>
   <si>
@@ -189,27 +168,12 @@
     <t>**Portions of the Util library were taken from open source. Those portions are marked as such.</t>
   </si>
   <si>
-    <t>*Source was taken from a post 2.3.2 release, includes portions of SFML 2.4.2 and 2.5.0 and has been modified</t>
-  </si>
-  <si>
     <t>Library</t>
   </si>
   <si>
     <t>Util**</t>
   </si>
   <si>
-    <t>gsl</t>
-  </si>
-  <si>
-    <t>Microsoft Guidelines Standard Library</t>
-  </si>
-  <si>
-    <t>MIT</t>
-  </si>
-  <si>
-    <t>https://github.com/Microsoft/GSL</t>
-  </si>
-  <si>
     <t>LZ4, OpenSSL, Util, RapidJSON, vcredist_x64, SQLite, gsl</t>
   </si>
   <si>
@@ -220,6 +184,18 @@
   </si>
   <si>
     <t>App</t>
+  </si>
+  <si>
+    <t>1.9.3</t>
+  </si>
+  <si>
+    <t>14.28.29914.0</t>
+  </si>
+  <si>
+    <t>Visual Studio 2019 (15.4.2) Runtimes</t>
+  </si>
+  <si>
+    <t>1.1.1k</t>
   </si>
 </sst>
 </file>
@@ -629,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -647,7 +623,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -673,7 +649,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>13</v>
@@ -682,7 +658,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -696,10 +672,10 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>17</v>
@@ -747,39 +723,39 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="5">
-        <v>2.19</v>
+        <v>35</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>32</v>
@@ -787,140 +763,95 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>38</v>
+      <c r="F8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" t="s">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4"/>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -930,14 +861,12 @@
     <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{5FBD2830-B6DE-4DAE-A79C-C871ABD3833F}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{EEA330EF-6A65-4581-BA95-F3510DA813A8}"/>
-    <hyperlink ref="F6" r:id="rId8" xr:uid="{4CF704C1-C1A0-413A-AAAC-6AAB65554510}"/>
-    <hyperlink ref="F11" r:id="rId9" xr:uid="{18342DE8-2680-4D4A-B473-D7A5378AED85}"/>
+    <hyperlink ref="F12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{EEA330EF-6A65-4581-BA95-F3510DA813A8}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{4CF704C1-C1A0-413A-AAAC-6AAB65554510}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>